<commit_message>
updated code to retrieve more articles
</commit_message>
<xml_diff>
--- a/more_grounding/retrived_maxo_annotations_df.xlsx
+++ b/more_grounding/retrived_maxo_annotations_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niyone/Desktop/maxo/automaxo/more_grounding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEC1C91-E88C-4C49-ADDC-C779D4CED6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB91340-0DC8-314E-A53C-653B3611DF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2703,8 +2703,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G69">
-    <sortCondition ref="A1:A69"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G68">
+    <sortCondition ref="A1:A68"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>